<commit_message>
add c++ json parsing and additions to sbc list and formations
</commit_message>
<xml_diff>
--- a/Data/SBC_List.xlsx
+++ b/Data/SBC_List.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ForbesLabs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ForbesLabs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315" xr2:uid="{1A7AE4BB-13F7-44DD-B191-6B524333BFA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -102,12 +102,21 @@
   </si>
   <si>
     <t>max same league</t>
+  </si>
+  <si>
+    <t>84-Rated Squad</t>
+  </si>
+  <si>
+    <t>Icons</t>
+  </si>
+  <si>
+    <t>Petit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,18 +461,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DBD0C7-77BE-46FB-BE72-913A7DEAA0D5}">
-  <dimension ref="A1:W5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -582,17 +590,40 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>41212</v>
+      </c>
+      <c r="P3">
+        <v>75</v>
+      </c>
+      <c r="Q3">
+        <v>84</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>11</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>11</v>
+      </c>
+      <c r="V3">
+        <v>11</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>